<commit_message>
results for 10 iterations
</commit_message>
<xml_diff>
--- a/Benchmark/File-stability/flippedResults.xlsx
+++ b/Benchmark/File-stability/flippedResults.xlsx
@@ -462,16 +462,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -481,16 +481,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -500,16 +500,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -538,13 +538,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -557,16 +557,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -576,16 +576,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -595,13 +595,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -614,13 +614,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -633,16 +633,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
@@ -652,16 +652,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14">
@@ -690,16 +690,16 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -709,16 +709,16 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" t="n">
+        <v>9</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
         <v>1</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -747,16 +747,16 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
@@ -766,16 +766,16 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -785,13 +785,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C19" t="n">
         <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
@@ -804,13 +804,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -823,13 +823,13 @@
         </is>
       </c>
       <c r="B21" t="n">
+        <v>14</v>
+      </c>
+      <c r="C21" t="n">
         <v>2</v>
       </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -842,16 +842,16 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -861,13 +861,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>

</xml_diff>